<commit_message>
minor bug fix + streamlit update
</commit_message>
<xml_diff>
--- a/data/admin_review_report.xlsx
+++ b/data/admin_review_report.xlsx
@@ -446,7 +446,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="33" customWidth="1" min="1" max="1"/>
+    <col width="31" customWidth="1" min="1" max="1"/>
     <col width="9" customWidth="1" min="2" max="2"/>
     <col width="23" customWidth="1" min="3" max="3"/>
   </cols>
@@ -486,7 +486,7 @@
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Appointments with Dr. Shreyansh</t>
+          <t>Appointments with Dr. Naresh</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
@@ -501,7 +501,7 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Appointments at Gachibowli</t>
+          <t>Appointments at Jubliee Hills</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
@@ -516,7 +516,7 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Patients with 12345</t>
+          <t>Patients with Aetna</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">

</xml_diff>

<commit_message>
feat : patient db update
</commit_message>
<xml_diff>
--- a/data/admin_review_report.xlsx
+++ b/data/admin_review_report.xlsx
@@ -446,7 +446,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="38" customWidth="1" min="1" max="1"/>
+    <col width="33" customWidth="1" min="1" max="1"/>
     <col width="9" customWidth="1" min="2" max="2"/>
     <col width="23" customWidth="1" min="3" max="3"/>
   </cols>
@@ -501,7 +501,7 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Appointments at Banjara Hills</t>
+          <t>Appointments at Jubliee Hills</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
@@ -516,7 +516,7 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Patients with Blue Cross Blue Shield</t>
+          <t>Patients with Aetna</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">

</xml_diff>

<commit_message>
feat : real email service
</commit_message>
<xml_diff>
--- a/data/admin_review_report.xlsx
+++ b/data/admin_review_report.xlsx
@@ -438,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,8 +446,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="33" customWidth="1" min="1" max="1"/>
-    <col width="9" customWidth="1" min="2" max="2"/>
+    <col width="38" customWidth="1" min="1" max="1"/>
+    <col width="11" customWidth="1" min="2" max="2"/>
     <col width="23" customWidth="1" min="3" max="3"/>
   </cols>
   <sheetData>
@@ -475,7 +475,7 @@
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
@@ -490,7 +490,7 @@
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="inlineStr">
         <is>
@@ -501,45 +501,180 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Appointments at Jubliee Hills</t>
+          <t>Appointments with Dr. Naveen</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Location Distribution</t>
+          <t>Doctor Distribution</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Patients with Aetna</t>
+          <t>Appointments with Dr. Aish</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Insurance Analysis</t>
+          <t>Doctor Distribution</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
+          <t>Appointments with Dr. Naresh</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Doctor Distribution</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>Appointments at Banjara Hills</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>Location Distribution</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>Appointments at Gachibowli</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>Location Distribution</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="inlineStr">
+        <is>
+          <t>Appointments at Jubliee Hills</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>Location Distribution</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>Patients with Aetna</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>Insurance Analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>Patients with Blue Cross Blue Shield</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>Insurance Analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>Patients with Cigna</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>Insurance Analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Patients with aetna</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>Insurance Analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Patients with cigna</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>Insurance Analysis</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
           <t>Estimated Revenue</t>
         </is>
       </c>
-      <c r="B6" s="2" t="inlineStr">
-        <is>
-          <t>$120.00</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>$1,020.00</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
         <is>
           <t>Financial</t>
         </is>

</xml_diff>